<commit_message>
debugged the matvaretabell_analysis GTG!
</commit_message>
<xml_diff>
--- a/data/auxillary/food_composition.xlsx
+++ b/data/auxillary/food_composition.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Categories</t>
+          <t>Main Category</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -492,31 +492,31 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.184444444444445</v>
+        <v>0.7868965517241379</v>
       </c>
       <c r="C2" t="n">
-        <v>1.695555555555555</v>
+        <v>0.5206896551724138</v>
       </c>
       <c r="D2" t="n">
-        <v>9.271111111111111</v>
+        <v>9.204137931034483</v>
       </c>
       <c r="E2" t="n">
-        <v>87.71111111111111</v>
+        <v>87.32638888888889</v>
       </c>
       <c r="F2" t="n">
-        <v>41.53333333333333</v>
+        <v>26.5</v>
       </c>
       <c r="G2" t="n">
-        <v>5.793333333333333</v>
+        <v>8.106206896551726</v>
       </c>
       <c r="H2" t="n">
-        <v>57.57777777777778</v>
+        <v>58.7448275862069</v>
       </c>
       <c r="I2" t="n">
         <v>100</v>
       </c>
       <c r="J2" t="n">
-        <v>12.28888888888889</v>
+        <v>12.67361111111111</v>
       </c>
     </row>
     <row r="3">
@@ -526,31 +526,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.783720930232558</v>
+        <v>11.17368421052632</v>
       </c>
       <c r="C3" t="n">
-        <v>9.513953488372094</v>
+        <v>8.25</v>
       </c>
       <c r="D3" t="n">
-        <v>15.78604651162791</v>
+        <v>25.12105263157895</v>
       </c>
       <c r="E3" t="n">
-        <v>68.48837209302326</v>
+        <v>33.05263157894737</v>
       </c>
       <c r="F3" t="n">
-        <v>94.07317073170732</v>
+        <v>249.3684210526316</v>
       </c>
       <c r="G3" t="n">
-        <v>12.71627906976744</v>
+        <v>6.850000000000001</v>
       </c>
       <c r="H3" t="n">
-        <v>171</v>
+        <v>264.921052631579</v>
       </c>
       <c r="I3" t="n">
-        <v>99.20930232558139</v>
+        <v>94.31578947368421</v>
       </c>
       <c r="J3" t="n">
-        <v>31.51162790697675</v>
+        <v>66.94736842105263</v>
       </c>
     </row>
     <row r="4">
@@ -560,31 +560,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9.303347280334728</v>
+        <v>11.74583333333333</v>
       </c>
       <c r="C4" t="n">
-        <v>14.7744769874477</v>
+        <v>14.54027777777778</v>
       </c>
       <c r="D4" t="n">
-        <v>13.99246861924686</v>
+        <v>5.888888888888889</v>
       </c>
       <c r="E4" t="n">
-        <v>61.08786610878661</v>
+        <v>67.6875</v>
       </c>
       <c r="F4" t="n">
-        <v>222.5188284518829</v>
+        <v>284.8333333333333</v>
       </c>
       <c r="G4" t="n">
-        <v>10.14309623430962</v>
+        <v>5.770138888888889</v>
       </c>
       <c r="H4" t="n">
-        <v>228.163179916318</v>
+        <v>201.6597222222222</v>
       </c>
       <c r="I4" t="n">
         <v>100</v>
       </c>
       <c r="J4" t="n">
-        <v>38.91213389121339</v>
+        <v>32.3125</v>
       </c>
     </row>
     <row r="5">
@@ -594,31 +594,31 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.77826086956522</v>
+        <v>12.56</v>
       </c>
       <c r="C5" t="n">
-        <v>10.88695652173913</v>
+        <v>13.23333333333333</v>
       </c>
       <c r="D5" t="n">
-        <v>12.85217391304348</v>
+        <v>1.926666666666667</v>
       </c>
       <c r="E5" t="n">
-        <v>64.78260869565217</v>
+        <v>72.33333333333333</v>
       </c>
       <c r="F5" t="n">
-        <v>180.5652173913043</v>
+        <v>211.8666666666667</v>
       </c>
       <c r="G5" t="n">
-        <v>4.026086956521739</v>
+        <v>1.92</v>
       </c>
       <c r="H5" t="n">
-        <v>193.4782608695652</v>
+        <v>177.0666666666667</v>
       </c>
       <c r="I5" t="n">
-        <v>97.91304347826087</v>
+        <v>96.8</v>
       </c>
       <c r="J5" t="n">
-        <v>35.21739130434783</v>
+        <v>27.66666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -628,31 +628,31 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13.35510204081633</v>
+        <v>15.62995594713656</v>
       </c>
       <c r="C6" t="n">
-        <v>5.169387755102041</v>
+        <v>7.644493392070484</v>
       </c>
       <c r="D6" t="n">
-        <v>5.26530612244898</v>
+        <v>4.531277533039647</v>
       </c>
       <c r="E6" t="n">
-        <v>75.58333333333333</v>
+        <v>71.66964285714286</v>
       </c>
       <c r="F6" t="n">
-        <v>168.1041666666667</v>
+        <v>194.4096916299559</v>
       </c>
       <c r="G6" t="n">
-        <v>1.448979591836735</v>
+        <v>1.165198237885463</v>
       </c>
       <c r="H6" t="n">
-        <v>122.0612244897959</v>
+        <v>150.1013215859031</v>
       </c>
       <c r="I6" t="n">
-        <v>92.93181818181819</v>
+        <v>88.98360655737704</v>
       </c>
       <c r="J6" t="n">
-        <v>24.41666666666667</v>
+        <v>28.33035714285714</v>
       </c>
     </row>
     <row r="7">
@@ -662,31 +662,31 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5.576712328767123</v>
+        <v>4.614364640883978</v>
       </c>
       <c r="C7" t="n">
-        <v>18.1513698630137</v>
+        <v>10.12099447513812</v>
       </c>
       <c r="D7" t="n">
-        <v>24.93561643835616</v>
+        <v>19.88397790055249</v>
       </c>
       <c r="E7" t="n">
-        <v>47.73287671232877</v>
+        <v>60.26519337016575</v>
       </c>
       <c r="F7" t="n">
-        <v>131.0616438356165</v>
+        <v>121.6850828729282</v>
       </c>
       <c r="G7" t="n">
-        <v>17.40547945205479</v>
+        <v>16.2939226519337</v>
       </c>
       <c r="H7" t="n">
-        <v>292.6712328767123</v>
+        <v>199.1436464088398</v>
       </c>
       <c r="I7" t="n">
-        <v>94.78620689655172</v>
+        <v>90.44692737430168</v>
       </c>
       <c r="J7" t="n">
-        <v>52.26712328767123</v>
+        <v>39.73480662983425</v>
       </c>
     </row>
     <row r="8">
@@ -696,31 +696,31 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8.753672316384181</v>
+        <v>7.895876288659793</v>
       </c>
       <c r="C8" t="n">
-        <v>5.089265536723164</v>
+        <v>9.149484536082474</v>
       </c>
       <c r="D8" t="n">
-        <v>42.35819209039548</v>
+        <v>49.45541237113402</v>
       </c>
       <c r="E8" t="n">
-        <v>39.15819209039548</v>
+        <v>28.59536082474227</v>
       </c>
       <c r="F8" t="n">
-        <v>175.8587570621469</v>
+        <v>182.9716494845361</v>
       </c>
       <c r="G8" t="n">
-        <v>4.521468926553672</v>
+        <v>11.57268041237113</v>
       </c>
       <c r="H8" t="n">
-        <v>259.6327683615819</v>
+        <v>321.6417525773196</v>
       </c>
       <c r="I8" t="n">
         <v>100</v>
       </c>
       <c r="J8" t="n">
-        <v>60.84180790960452</v>
+        <v>71.40463917525773</v>
       </c>
     </row>
     <row r="9">
@@ -730,31 +730,31 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9.520000000000001</v>
+        <v>13.90645161290323</v>
       </c>
       <c r="C9" t="n">
-        <v>3.163333333333334</v>
+        <v>1.990322580645161</v>
       </c>
       <c r="D9" t="n">
-        <v>18.48333333333333</v>
+        <v>24.88387096774193</v>
       </c>
       <c r="E9" t="n">
-        <v>62.6</v>
+        <v>50.54838709677419</v>
       </c>
       <c r="F9" t="n">
-        <v>157.728813559322</v>
+        <v>222.3225806451613</v>
       </c>
       <c r="G9" t="n">
-        <v>4.093333333333333</v>
+        <v>2.7</v>
       </c>
       <c r="H9" t="n">
-        <v>153.2166666666667</v>
+        <v>190.6451612903226</v>
       </c>
       <c r="I9" t="n">
-        <v>98.68333333333334</v>
+        <v>99.64516129032258</v>
       </c>
       <c r="J9" t="n">
-        <v>37.4</v>
+        <v>49.45161290322581</v>
       </c>
     </row>
     <row r="10">
@@ -764,201 +764,167 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8.411308203991132</v>
+        <v>6.017021276595744</v>
       </c>
       <c r="C10" t="n">
-        <v>11.09722838137472</v>
+        <v>22.48662613981763</v>
       </c>
       <c r="D10" t="n">
-        <v>17.51230598669623</v>
+        <v>13.8258358662614</v>
       </c>
       <c r="E10" t="n">
-        <v>59.31549609810479</v>
+        <v>55.55487804878049</v>
       </c>
       <c r="F10" t="n">
-        <v>150.9574468085106</v>
+        <v>127.0501567398119</v>
       </c>
       <c r="G10" t="n">
-        <v>7.249109131403118</v>
+        <v>4.196625766871166</v>
       </c>
       <c r="H10" t="n">
-        <v>212.4460511679644</v>
+        <v>288.7055214723927</v>
       </c>
       <c r="I10" t="n">
-        <v>95.10606060606061</v>
+        <v>100</v>
       </c>
       <c r="J10" t="n">
-        <v>40.68450390189521</v>
+        <v>44.44512195121951</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Poultry</t>
+          <t>Red meat</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>18.79130434782609</v>
+        <v>18.39186046511628</v>
       </c>
       <c r="C11" t="n">
-        <v>8.32391304347826</v>
+        <v>11.73875968992248</v>
       </c>
       <c r="D11" t="n">
-        <v>3.673913043478261</v>
+        <v>2.857364341085272</v>
       </c>
       <c r="E11" t="n">
-        <v>68.91304347826087</v>
+        <v>66.67829457364341</v>
       </c>
       <c r="F11" t="n">
-        <v>203.3260869565217</v>
+        <v>196.9182879377432</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3239130434782609</v>
+        <v>0.6833333333333333</v>
       </c>
       <c r="H11" t="n">
-        <v>165.3478260869565</v>
+        <v>191.3759689922481</v>
       </c>
       <c r="I11" t="n">
-        <v>89.90909090909091</v>
+        <v>97.33070866141732</v>
       </c>
       <c r="J11" t="n">
-        <v>31.08695652173913</v>
+        <v>33.32170542635659</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Red meat</t>
+          <t>Starchy vegetables</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>18.2408</v>
+        <v>2.323529411764706</v>
       </c>
       <c r="C12" t="n">
-        <v>9.843999999999999</v>
+        <v>5.8</v>
       </c>
       <c r="D12" t="n">
-        <v>3.0272</v>
+        <v>18.73529411764706</v>
       </c>
       <c r="E12" t="n">
-        <v>68.52</v>
+        <v>70.47058823529412</v>
       </c>
       <c r="F12" t="n">
-        <v>178.88</v>
+        <v>72.41176470588235</v>
       </c>
       <c r="G12" t="n">
-        <v>0.6207999999999999</v>
+        <v>2.170588235294117</v>
       </c>
       <c r="H12" t="n">
-        <v>174.472</v>
+        <v>140.4117647058823</v>
       </c>
       <c r="I12" t="n">
-        <v>98.44354838709677</v>
+        <v>96.11764705882354</v>
       </c>
       <c r="J12" t="n">
-        <v>31.48</v>
+        <v>29.52941176470588</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Starchy vegetables</t>
+          <t>Sweets and snacks</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.5475</v>
+        <v>3.512903225806452</v>
       </c>
       <c r="C13" t="n">
-        <v>7.5525</v>
+        <v>9.835483870967741</v>
       </c>
       <c r="D13" t="n">
-        <v>24.465</v>
+        <v>20.18064516129032</v>
       </c>
       <c r="E13" t="n">
-        <v>61.2</v>
+        <v>64.83870967741936</v>
       </c>
       <c r="F13" t="n">
-        <v>85.825</v>
+        <v>102.6451612903226</v>
       </c>
       <c r="G13" t="n">
-        <v>2.375</v>
+        <v>18.70645161290323</v>
       </c>
       <c r="H13" t="n">
-        <v>185.775</v>
+        <v>186.7741935483871</v>
       </c>
       <c r="I13" t="n">
-        <v>97.65000000000001</v>
+        <v>100</v>
       </c>
       <c r="J13" t="n">
-        <v>38.8</v>
+        <v>35.16129032258065</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Sweets and snacks</t>
+          <t>Vegetables</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3.893814432989691</v>
+        <v>2.003164556962025</v>
       </c>
       <c r="C14" t="n">
-        <v>10.06185567010309</v>
+        <v>1.654430379746836</v>
       </c>
       <c r="D14" t="n">
-        <v>40.94226804123711</v>
+        <v>5.648101265822785</v>
       </c>
       <c r="E14" t="n">
-        <v>41.79381443298969</v>
+        <v>87.91082802547771</v>
       </c>
       <c r="F14" t="n">
-        <v>88.61855670103093</v>
+        <v>50.28481012658228</v>
       </c>
       <c r="G14" t="n">
-        <v>28.14639175257732</v>
+        <v>3.557961783439491</v>
       </c>
       <c r="H14" t="n">
-        <v>280.5876288659794</v>
+        <v>51.03797468354431</v>
       </c>
       <c r="I14" t="n">
-        <v>98.68041237113403</v>
+        <v>89.52903225806452</v>
       </c>
       <c r="J14" t="n">
-        <v>58.20618556701031</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Vegetables</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>4.052631578947368</v>
-      </c>
-      <c r="C15" t="n">
-        <v>15.82631578947368</v>
-      </c>
-      <c r="D15" t="n">
-        <v>7.052631578947368</v>
-      </c>
-      <c r="E15" t="n">
-        <v>71.73684210526316</v>
-      </c>
-      <c r="F15" t="n">
-        <v>61.94736842105263</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1.921052631578947</v>
-      </c>
-      <c r="H15" t="n">
-        <v>189.5263157894737</v>
-      </c>
-      <c r="I15" t="n">
-        <v>98.56140350877193</v>
-      </c>
-      <c r="J15" t="n">
-        <v>28.26315789473684</v>
+        <v>12.08917197452229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done with food pyramids
</commit_message>
<xml_diff>
--- a/data/auxillary/food_composition.xlsx
+++ b/data/auxillary/food_composition.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Main Category</t>
+          <t>Category</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -798,132 +798,166 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>18.39186046511628</v>
+        <v>19.41290322580645</v>
       </c>
       <c r="C11" t="n">
-        <v>11.73875968992248</v>
+        <v>9.129032258064516</v>
       </c>
       <c r="D11" t="n">
-        <v>2.857364341085272</v>
+        <v>2.474193548387097</v>
       </c>
       <c r="E11" t="n">
-        <v>66.67829457364341</v>
+        <v>68.74193548387096</v>
       </c>
       <c r="F11" t="n">
-        <v>196.9182879377432</v>
+        <v>204.5322580645161</v>
       </c>
       <c r="G11" t="n">
-        <v>0.6833333333333333</v>
+        <v>0.4</v>
       </c>
       <c r="H11" t="n">
-        <v>191.3759689922481</v>
+        <v>170.1774193548387</v>
       </c>
       <c r="I11" t="n">
-        <v>97.33070866141732</v>
+        <v>92.34482758620689</v>
       </c>
       <c r="J11" t="n">
-        <v>33.32170542635659</v>
+        <v>31.25806451612903</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Starchy vegetables</t>
+          <t>Red meat</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2.323529411764706</v>
+        <v>18.06887755102041</v>
       </c>
       <c r="C12" t="n">
-        <v>5.8</v>
+        <v>12.56428571428571</v>
       </c>
       <c r="D12" t="n">
-        <v>18.73529411764706</v>
+        <v>2.978571428571428</v>
       </c>
       <c r="E12" t="n">
-        <v>70.47058823529412</v>
+        <v>66.02551020408163</v>
       </c>
       <c r="F12" t="n">
-        <v>72.41176470588235</v>
+        <v>194.4974358974359</v>
       </c>
       <c r="G12" t="n">
-        <v>2.170588235294117</v>
+        <v>0.7729591836734694</v>
       </c>
       <c r="H12" t="n">
-        <v>140.4117647058823</v>
+        <v>198.0816326530612</v>
       </c>
       <c r="I12" t="n">
-        <v>96.11764705882354</v>
+        <v>98.80612244897959</v>
       </c>
       <c r="J12" t="n">
-        <v>29.52941176470588</v>
+        <v>33.97448979591837</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Sweets and snacks</t>
+          <t>Starchy vegetables</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.512903225806452</v>
+        <v>2.323529411764706</v>
       </c>
       <c r="C13" t="n">
-        <v>9.835483870967741</v>
+        <v>5.8</v>
       </c>
       <c r="D13" t="n">
-        <v>20.18064516129032</v>
+        <v>18.73529411764706</v>
       </c>
       <c r="E13" t="n">
-        <v>64.83870967741936</v>
+        <v>70.47058823529412</v>
       </c>
       <c r="F13" t="n">
-        <v>102.6451612903226</v>
+        <v>72.41176470588235</v>
       </c>
       <c r="G13" t="n">
-        <v>18.70645161290323</v>
+        <v>2.170588235294117</v>
       </c>
       <c r="H13" t="n">
-        <v>186.7741935483871</v>
+        <v>140.4117647058823</v>
       </c>
       <c r="I13" t="n">
-        <v>100</v>
+        <v>96.11764705882354</v>
       </c>
       <c r="J13" t="n">
-        <v>35.16129032258065</v>
+        <v>29.52941176470588</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
+          <t>Sweets and snacks</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3.512903225806452</v>
+      </c>
+      <c r="C14" t="n">
+        <v>9.835483870967741</v>
+      </c>
+      <c r="D14" t="n">
+        <v>20.18064516129032</v>
+      </c>
+      <c r="E14" t="n">
+        <v>64.83870967741936</v>
+      </c>
+      <c r="F14" t="n">
+        <v>102.6451612903226</v>
+      </c>
+      <c r="G14" t="n">
+        <v>18.70645161290323</v>
+      </c>
+      <c r="H14" t="n">
+        <v>186.7741935483871</v>
+      </c>
+      <c r="I14" t="n">
+        <v>100</v>
+      </c>
+      <c r="J14" t="n">
+        <v>35.16129032258065</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
           <t>Vegetables</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="B15" t="n">
         <v>2.003164556962025</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C15" t="n">
         <v>1.654430379746836</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>5.648101265822785</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E15" t="n">
         <v>87.91082802547771</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F15" t="n">
         <v>50.28481012658228</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G15" t="n">
         <v>3.557961783439491</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H15" t="n">
         <v>51.03797468354431</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I15" t="n">
         <v>89.52903225806452</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J15" t="n">
         <v>12.08917197452229</v>
       </c>
     </row>

</xml_diff>